<commit_message>
Add excel file that compares data between sql
</commit_message>
<xml_diff>
--- a/analysis/total_subscribers_analysis.xlsx
+++ b/analysis/total_subscribers_analysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chaem\Dropbox\My PC (DESKTOP-UI9CKON)\Desktop\NOV 2024 - BackUpFolder\Coding Projects\Data Analytics Projects\0b.-SSMS-World-Wide-Youtube-Channel-Analytics-Project-Walkthrough-\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chaem\Dropbox\My PC (DESKTOP-UI9CKON)\Desktop\NOV 2024 - BackUpFolder\Coding Projects\Data Analytics Projects\0b.-SSMS-World-Wide-Youtube-Channel-Analytics-Project-Walkthrough-\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2EFCB18-0DC2-4A4C-981E-638663DB6271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB4A6563-F5CD-4B79-BB02-E0742D79DF24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6420" yWindow="0" windowWidth="22485" windowHeight="15585" xr2:uid="{5D8DE40C-5D99-4416-ABEA-3623E34DD1C8}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{5D8DE40C-5D99-4416-ABEA-3623E34DD1C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -119,7 +119,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="172" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -258,9 +258,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -282,48 +279,37 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
@@ -692,7 +678,7 @@
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -716,259 +702,259 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="24" x14ac:dyDescent="0.4">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="A1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>0.02</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="10">
         <v>50000</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="21" x14ac:dyDescent="0.35">
-      <c r="N8" s="14" t="s">
+      <c r="N8" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="14"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="16"/>
     </row>
     <row r="9" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="H9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="I9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="J9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N9" s="7" t="s">
+      <c r="N9" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="O9" s="6" t="s">
+      <c r="O9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="P9" s="8" t="s">
+      <c r="P9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="Q9" s="9" t="s">
+      <c r="Q9" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="10">
         <v>135200</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="10">
         <v>135200</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="12">
         <f>B10*D4</f>
         <v>2704</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="10">
         <v>2704</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10" s="12">
         <f>D10*D5</f>
         <v>13520</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="10">
         <v>13520</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="12">
         <f>F10-D6</f>
         <v>-36480</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="10">
         <v>-36480</v>
       </c>
-      <c r="J10" s="5">
+      <c r="J10" s="4">
         <f>H10-I10</f>
         <v>0</v>
       </c>
-      <c r="N10" s="13">
+      <c r="N10" s="12">
         <f>B10-C10</f>
         <v>0</v>
       </c>
-      <c r="O10" s="13">
+      <c r="O10" s="12">
         <f>D10-E10</f>
         <v>0</v>
       </c>
-      <c r="P10" s="13">
+      <c r="P10" s="12">
         <f>F10-G10</f>
         <v>0</v>
       </c>
-      <c r="Q10" s="13">
+      <c r="Q10" s="12">
         <f>H10-I10</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="11">
         <v>104000000</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="11">
         <v>104000000</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="12">
         <f>B11*D4</f>
         <v>2080000</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="10">
         <v>2080000</v>
       </c>
-      <c r="F11" s="13">
+      <c r="F11" s="12">
         <f>D11*D5</f>
         <v>10400000</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="10">
         <v>10400000</v>
       </c>
-      <c r="H11" s="15">
+      <c r="H11" s="13">
         <v>10350000</v>
       </c>
-      <c r="I11" s="15">
+      <c r="I11" s="13">
         <v>10350000</v>
       </c>
-      <c r="J11" s="13">
+      <c r="J11" s="12">
         <f>H11-I11</f>
         <v>0</v>
       </c>
-      <c r="N11" s="13">
+      <c r="N11" s="12">
         <f t="shared" ref="N11:N12" si="0">B11-C11</f>
         <v>0</v>
       </c>
-      <c r="O11" s="13">
+      <c r="O11" s="12">
         <f t="shared" ref="O11:O12" si="1">D11-E11</f>
         <v>0</v>
       </c>
-      <c r="P11" s="13">
+      <c r="P11" s="12">
         <f t="shared" ref="P11:P12" si="2">F11-G11</f>
         <v>0</v>
       </c>
-      <c r="Q11" s="13">
+      <c r="Q11" s="12">
         <f t="shared" ref="Q11:Q12" si="3">H11-I11</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12" s="11">
         <v>5100000</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="11">
         <v>5100000</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="12">
         <f>B12*D4</f>
         <v>102000</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E12" s="10">
         <v>102000</v>
       </c>
-      <c r="F12" s="13">
+      <c r="F12" s="12">
         <f>D12*D5</f>
         <v>510000</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="10">
         <v>510000</v>
       </c>
-      <c r="H12" s="11">
+      <c r="H12" s="10">
         <v>460000</v>
       </c>
-      <c r="I12" s="11">
+      <c r="I12" s="10">
         <v>460000</v>
       </c>
-      <c r="J12" s="11">
+      <c r="J12" s="10">
         <f>H12-I12</f>
         <v>0</v>
       </c>
-      <c r="N12" s="13">
+      <c r="N12" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O12" s="13">
+      <c r="O12" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P12" s="13">
+      <c r="P12" s="12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q12" s="13">
+      <c r="Q12" s="12">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="14" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>